<commit_message>
Update Modelo de Dominio + Expecificaçoes de UC
-Alteração ao modelo de Domínio( vpp e imagem )
-Especificação do Gestor de Exercícios 20%
-Pequena mudança Especificação do Gestor de notificações
</commit_message>
<xml_diff>
--- a/Diagramas de UC e Especificações Textuais/2-Especificação do gestor de notificações.xlsx
+++ b/Diagramas de UC e Especificações Textuais/2-Especificação do gestor de notificações.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RS\Documents\GitHub\EAW_MEI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RS\Documents\GitHub\EAW_MEI\Diagramas de UC e Especificações Textuais\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -858,112 +858,10 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -972,34 +870,16 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1009,6 +889,42 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1016,6 +932,90 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1300,7 +1300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -1317,52 +1317,52 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="95" t="s">
+      <c r="B2" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="52" t="s">
+      <c r="C2" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="74"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="95" t="s">
+      <c r="B3" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="57"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77"/>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="75" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="57"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="77"/>
     </row>
     <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="95" t="s">
+      <c r="B5" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="58"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="80"/>
     </row>
     <row r="6" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="81" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="96"/>
+      <c r="C6" s="59"/>
       <c r="D6" s="12" t="s">
         <v>5</v>
       </c>
@@ -1378,8 +1378,8 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="101"/>
-      <c r="C7" s="97">
+      <c r="B7" s="82"/>
+      <c r="C7" s="60">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -1390,13 +1390,13 @@
       <c r="G7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="72" t="s">
+      <c r="H7" s="87" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="101"/>
-      <c r="C8" s="97"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="60"/>
       <c r="D8" s="4"/>
       <c r="E8" s="5">
         <v>2</v>
@@ -1407,11 +1407,11 @@
       <c r="G8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="72"/>
+      <c r="H8" s="87"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="101"/>
-      <c r="C9" s="97"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="60"/>
       <c r="D9" s="4"/>
       <c r="E9" s="5">
         <v>3</v>
@@ -1422,11 +1422,11 @@
       <c r="G9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="72"/>
+      <c r="H9" s="87"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="101"/>
-      <c r="C10" s="98">
+      <c r="B10" s="82"/>
+      <c r="C10" s="61">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -1437,13 +1437,13 @@
       <c r="G10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="66" t="s">
+      <c r="H10" s="88" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="101"/>
-      <c r="C11" s="98"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="2"/>
       <c r="E11" s="3">
         <v>5</v>
@@ -1454,11 +1454,11 @@
       <c r="G11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="67"/>
+      <c r="H11" s="89"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="101"/>
-      <c r="C12" s="98"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="2"/>
       <c r="E12" s="3">
         <v>6</v>
@@ -1469,11 +1469,11 @@
       <c r="G12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="67"/>
+      <c r="H12" s="89"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="101"/>
-      <c r="C13" s="98"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="2"/>
       <c r="E13" s="3">
         <v>7</v>
@@ -1484,11 +1484,11 @@
       <c r="G13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="67"/>
+      <c r="H13" s="89"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="102"/>
-      <c r="C14" s="99"/>
+      <c r="B14" s="83"/>
+      <c r="C14" s="62"/>
       <c r="D14" s="6"/>
       <c r="E14" s="7">
         <v>8</v>
@@ -1497,13 +1497,13 @@
         <v>35</v>
       </c>
       <c r="G14" s="6"/>
-      <c r="H14" s="67"/>
+      <c r="H14" s="89"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="100" t="s">
+      <c r="B15" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="103" t="s">
+      <c r="C15" s="63" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="15" t="s">
@@ -1514,54 +1514,54 @@
       <c r="G15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="46" t="s">
+      <c r="H15" s="93" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="101"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="81"/>
-      <c r="E16" s="80" t="s">
+      <c r="B16" s="82"/>
+      <c r="C16" s="64"/>
+      <c r="D16" s="47"/>
+      <c r="E16" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="F16" s="81" t="s">
+      <c r="F16" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G16" s="81"/>
-      <c r="H16" s="47"/>
+      <c r="G16" s="47"/>
+      <c r="H16" s="94"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="101"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="81"/>
-      <c r="E17" s="80" t="s">
+      <c r="B17" s="82"/>
+      <c r="C17" s="64"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="81" t="s">
+      <c r="F17" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="G17" s="81"/>
-      <c r="H17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="94"/>
     </row>
     <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="102"/>
-      <c r="C18" s="105"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="74" t="s">
+      <c r="B18" s="83"/>
+      <c r="C18" s="65"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="F18" s="83" t="s">
+      <c r="F18" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="G18" s="75"/>
-      <c r="H18" s="48"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="95"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="103" t="s">
+      <c r="C19" s="63" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="15" t="s">
@@ -1572,132 +1572,132 @@
       <c r="G19" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="46" t="s">
+      <c r="H19" s="93" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="101"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="81"/>
-      <c r="E20" s="80" t="s">
+      <c r="B20" s="82"/>
+      <c r="C20" s="64"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="F20" s="81" t="s">
+      <c r="F20" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="81"/>
-      <c r="H20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="94"/>
     </row>
     <row r="21" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="102"/>
-      <c r="C21" s="106"/>
+      <c r="B21" s="83"/>
+      <c r="C21" s="66"/>
       <c r="D21" s="17"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="82" t="s">
+      <c r="F21" s="48" t="s">
         <v>81</v>
       </c>
       <c r="G21" s="17"/>
-      <c r="H21" s="48"/>
+      <c r="H21" s="95"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="100" t="s">
+      <c r="B22" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="107"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="84" t="s">
+      <c r="C22" s="67"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="86" t="s">
+      <c r="F22" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="G22" s="85"/>
-      <c r="H22" s="87" t="s">
+      <c r="G22" s="51"/>
+      <c r="H22" s="90" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="101"/>
-      <c r="C23" s="108"/>
-      <c r="D23" s="77"/>
-      <c r="E23" s="76" t="s">
+      <c r="B23" s="82"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F23" s="77" t="s">
+      <c r="F23" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="77" t="s">
+      <c r="G23" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="H23" s="78"/>
+      <c r="H23" s="91"/>
     </row>
     <row r="24" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="102"/>
-      <c r="C24" s="109"/>
+      <c r="B24" s="83"/>
+      <c r="C24" s="69"/>
       <c r="D24" s="9"/>
       <c r="E24" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="F24" s="79" t="s">
+      <c r="F24" s="45" t="s">
         <v>35</v>
       </c>
       <c r="G24" s="9"/>
-      <c r="H24" s="73"/>
+      <c r="H24" s="92"/>
     </row>
     <row r="25" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
       <c r="E25" s="1"/>
     </row>
     <row r="26" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="95" t="s">
+      <c r="B26" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="54"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="74"/>
     </row>
     <row r="27" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="95" t="s">
+      <c r="B27" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C27" s="55" t="s">
+      <c r="C27" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="56"/>
-      <c r="E27" s="56"/>
-      <c r="F27" s="57"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
     </row>
     <row r="28" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="95" t="s">
+      <c r="B28" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="55" t="s">
+      <c r="C28" s="75" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="57"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="77"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="95" t="s">
+      <c r="B29" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C29" s="58" t="s">
+      <c r="C29" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="59"/>
-      <c r="E29" s="59"/>
-      <c r="F29" s="60"/>
+      <c r="D29" s="79"/>
+      <c r="E29" s="79"/>
+      <c r="F29" s="80"/>
     </row>
     <row r="30" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="112" t="s">
+      <c r="B30" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="C30" s="96"/>
+      <c r="C30" s="59"/>
       <c r="D30" s="12" t="s">
         <v>5</v>
       </c>
@@ -1713,25 +1713,25 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="113"/>
-      <c r="C31" s="110">
+      <c r="B31" s="85"/>
+      <c r="C31" s="70">
         <v>0</v>
       </c>
-      <c r="D31" s="89" t="s">
+      <c r="D31" s="54" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="88"/>
+      <c r="E31" s="53"/>
       <c r="F31" s="23"/>
       <c r="G31" s="23"/>
-      <c r="H31" s="93" t="s">
+      <c r="H31" s="113" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="113"/>
-      <c r="C32" s="110"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="70"/>
       <c r="D32" s="23"/>
-      <c r="E32" s="88">
+      <c r="E32" s="53">
         <v>1</v>
       </c>
       <c r="F32" s="23" t="s">
@@ -1740,13 +1740,13 @@
       <c r="G32" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H32" s="93"/>
+      <c r="H32" s="113"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="113"/>
-      <c r="C33" s="110"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="70"/>
       <c r="D33" s="23"/>
-      <c r="E33" s="88">
+      <c r="E33" s="53">
         <v>2</v>
       </c>
       <c r="F33" s="23" t="s">
@@ -1755,13 +1755,13 @@
       <c r="G33" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="93"/>
+      <c r="H33" s="113"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="113"/>
-      <c r="C34" s="110"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="70"/>
       <c r="D34" s="23"/>
-      <c r="E34" s="88">
+      <c r="E34" s="53">
         <v>3</v>
       </c>
       <c r="F34" s="23" t="s">
@@ -1770,13 +1770,13 @@
       <c r="G34" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="93"/>
+      <c r="H34" s="113"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="113"/>
-      <c r="C35" s="110"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="70"/>
       <c r="D35" s="23"/>
-      <c r="E35" s="88">
+      <c r="E35" s="53">
         <v>4</v>
       </c>
       <c r="F35" s="23" t="s">
@@ -1785,20 +1785,20 @@
       <c r="G35" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H35" s="93"/>
+      <c r="H35" s="113"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="114"/>
-      <c r="C36" s="111"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="90">
+      <c r="B36" s="86"/>
+      <c r="C36" s="71"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="55">
         <v>5</v>
       </c>
-      <c r="F36" s="92" t="s">
+      <c r="F36" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="G36" s="91"/>
-      <c r="H36" s="94"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="114"/>
     </row>
     <row r="37" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
@@ -1813,59 +1813,59 @@
     </row>
     <row r="38" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="18"/>
-      <c r="B38" s="95" t="s">
+      <c r="B38" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="C38" s="52" t="s">
+      <c r="C38" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="53"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="54"/>
+      <c r="D38" s="73"/>
+      <c r="E38" s="73"/>
+      <c r="F38" s="74"/>
       <c r="I38" s="18"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="18"/>
-      <c r="B39" s="95" t="s">
+      <c r="B39" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="55" t="s">
+      <c r="C39" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="56"/>
-      <c r="F39" s="57"/>
+      <c r="D39" s="76"/>
+      <c r="E39" s="76"/>
+      <c r="F39" s="77"/>
       <c r="I39" s="18"/>
     </row>
     <row r="40" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
-      <c r="B40" s="95" t="s">
+      <c r="B40" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="C40" s="55" t="s">
+      <c r="C40" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="D40" s="56"/>
-      <c r="E40" s="56"/>
-      <c r="F40" s="57"/>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="77"/>
       <c r="I40" s="18"/>
     </row>
     <row r="41" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
-      <c r="B41" s="95" t="s">
+      <c r="B41" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="C41" s="58" t="s">
+      <c r="C41" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="D41" s="59"/>
-      <c r="E41" s="59"/>
-      <c r="F41" s="60"/>
+      <c r="D41" s="79"/>
+      <c r="E41" s="79"/>
+      <c r="F41" s="80"/>
       <c r="I41" s="18"/>
     </row>
     <row r="42" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
-      <c r="B42" s="61" t="s">
+      <c r="B42" s="104" t="s">
         <v>4</v>
       </c>
       <c r="C42" s="19"/>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
-      <c r="B43" s="62"/>
+      <c r="B43" s="105"/>
       <c r="C43" s="10">
         <v>1</v>
       </c>
@@ -1898,14 +1898,14 @@
       <c r="G43" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="H43" s="63" t="s">
+      <c r="H43" s="106" t="s">
         <v>18</v>
       </c>
       <c r="I43" s="18"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
-      <c r="B44" s="62"/>
+      <c r="B44" s="105"/>
       <c r="C44" s="10"/>
       <c r="D44" s="4"/>
       <c r="E44" s="5">
@@ -1917,12 +1917,12 @@
       <c r="G44" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H44" s="64"/>
+      <c r="H44" s="107"/>
       <c r="I44" s="18"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
-      <c r="B45" s="62"/>
+      <c r="B45" s="105"/>
       <c r="C45" s="10"/>
       <c r="D45" s="4"/>
       <c r="E45" s="5">
@@ -1934,12 +1934,12 @@
       <c r="G45" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H45" s="64"/>
+      <c r="H45" s="107"/>
       <c r="I45" s="18"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
-      <c r="B46" s="62"/>
+      <c r="B46" s="105"/>
       <c r="C46" s="10"/>
       <c r="D46" s="4"/>
       <c r="E46" s="5">
@@ -1951,12 +1951,12 @@
       <c r="G46" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H46" s="65"/>
+      <c r="H46" s="108"/>
       <c r="I46" s="18"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
-      <c r="B47" s="62"/>
+      <c r="B47" s="105"/>
       <c r="C47" s="11">
         <v>5</v>
       </c>
@@ -1968,14 +1968,14 @@
       <c r="G47" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="H47" s="66" t="s">
+      <c r="H47" s="88" t="s">
         <v>19</v>
       </c>
       <c r="I47" s="18"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
-      <c r="B48" s="62"/>
+      <c r="B48" s="105"/>
       <c r="C48" s="11"/>
       <c r="D48" s="2"/>
       <c r="E48" s="3">
@@ -1987,12 +1987,12 @@
       <c r="G48" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H48" s="67"/>
+      <c r="H48" s="89"/>
       <c r="I48" s="18"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
-      <c r="B49" s="62"/>
+      <c r="B49" s="105"/>
       <c r="C49" s="11"/>
       <c r="D49" s="2"/>
       <c r="E49" s="3">
@@ -2004,12 +2004,12 @@
       <c r="G49" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H49" s="68"/>
+      <c r="H49" s="109"/>
       <c r="I49" s="18"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
-      <c r="B50" s="62"/>
+      <c r="B50" s="105"/>
       <c r="C50" s="21">
         <v>8</v>
       </c>
@@ -2021,14 +2021,14 @@
       <c r="G50" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="H50" s="69" t="s">
+      <c r="H50" s="110" t="s">
         <v>66</v>
       </c>
       <c r="I50" s="18"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
-      <c r="B51" s="62"/>
+      <c r="B51" s="105"/>
       <c r="C51" s="21"/>
       <c r="D51" s="22"/>
       <c r="E51" s="24">
@@ -2040,12 +2040,12 @@
       <c r="G51" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="H51" s="70"/>
+      <c r="H51" s="111"/>
       <c r="I51" s="18"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
-      <c r="B52" s="62"/>
+      <c r="B52" s="105"/>
       <c r="C52" s="21"/>
       <c r="D52" s="22"/>
       <c r="E52" s="24">
@@ -2057,12 +2057,12 @@
       <c r="G52" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="H52" s="71"/>
+      <c r="H52" s="112"/>
       <c r="I52" s="18"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="18"/>
-      <c r="B53" s="62"/>
+      <c r="B53" s="105"/>
       <c r="C53" s="25">
         <v>11</v>
       </c>
@@ -2074,14 +2074,14 @@
       <c r="G53" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="H53" s="41" t="s">
+      <c r="H53" s="96" t="s">
         <v>67</v>
       </c>
       <c r="I53" s="18"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="18"/>
-      <c r="B54" s="62"/>
+      <c r="B54" s="105"/>
       <c r="C54" s="25"/>
       <c r="D54" s="26"/>
       <c r="E54" s="27">
@@ -2093,12 +2093,12 @@
       <c r="G54" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="H54" s="42"/>
+      <c r="H54" s="97"/>
       <c r="I54" s="18"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="18"/>
-      <c r="B55" s="62"/>
+      <c r="B55" s="105"/>
       <c r="C55" s="25"/>
       <c r="D55" s="26"/>
       <c r="E55" s="27">
@@ -2110,12 +2110,12 @@
       <c r="G55" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="H55" s="42"/>
+      <c r="H55" s="97"/>
       <c r="I55" s="18"/>
     </row>
     <row r="56" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
-      <c r="B56" s="62"/>
+      <c r="B56" s="105"/>
       <c r="C56" s="30"/>
       <c r="D56" s="31"/>
       <c r="E56" s="32">
@@ -2125,12 +2125,12 @@
         <v>35</v>
       </c>
       <c r="G56" s="31"/>
-      <c r="H56" s="42"/>
+      <c r="H56" s="97"/>
       <c r="I56" s="18"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
-      <c r="B57" s="43" t="s">
+      <c r="B57" s="98" t="s">
         <v>36</v>
       </c>
       <c r="C57" s="39" t="s">
@@ -2142,14 +2142,14 @@
       <c r="E57" s="39"/>
       <c r="F57" s="40"/>
       <c r="G57" s="40"/>
-      <c r="H57" s="49" t="s">
+      <c r="H57" s="101" t="s">
         <v>28</v>
       </c>
       <c r="I57" s="18"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="18"/>
-      <c r="B58" s="44"/>
+      <c r="B58" s="99"/>
       <c r="C58" s="29"/>
       <c r="D58" s="28"/>
       <c r="E58" s="29" t="s">
@@ -2161,12 +2161,12 @@
       <c r="G58" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H58" s="50"/>
+      <c r="H58" s="102"/>
       <c r="I58" s="18"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="18"/>
-      <c r="B59" s="44"/>
+      <c r="B59" s="99"/>
       <c r="C59" s="29"/>
       <c r="D59" s="28"/>
       <c r="E59" s="29" t="s">
@@ -2178,12 +2178,12 @@
       <c r="G59" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="H59" s="50"/>
+      <c r="H59" s="102"/>
       <c r="I59" s="18"/>
     </row>
     <row r="60" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
-      <c r="B60" s="45"/>
+      <c r="B60" s="100"/>
       <c r="C60" s="36"/>
       <c r="D60" s="34"/>
       <c r="E60" s="36" t="s">
@@ -2193,7 +2193,7 @@
         <v>74</v>
       </c>
       <c r="G60" s="34"/>
-      <c r="H60" s="51"/>
+      <c r="H60" s="103"/>
       <c r="I60" s="18"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -2544,11 +2544,17 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="H53:H56"/>
+    <mergeCell ref="B57:B60"/>
+    <mergeCell ref="H57:H60"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C39:F39"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="B42:B56"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="H47:H49"/>
+    <mergeCell ref="H50:H52"/>
     <mergeCell ref="B30:B36"/>
     <mergeCell ref="H7:H9"/>
     <mergeCell ref="H10:H14"/>
@@ -2560,20 +2566,14 @@
     <mergeCell ref="B15:B18"/>
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B22:B24"/>
-    <mergeCell ref="H53:H56"/>
-    <mergeCell ref="B57:B60"/>
-    <mergeCell ref="H57:H60"/>
-    <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C39:F39"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="B42:B56"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="H47:H49"/>
-    <mergeCell ref="H50:H52"/>
     <mergeCell ref="C28:F28"/>
     <mergeCell ref="C29:F29"/>
     <mergeCell ref="H31:H36"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="B6:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>